<commit_message>
new database changed added
</commit_message>
<xml_diff>
--- a/database/seeds/common_code.xlsx
+++ b/database/seeds/common_code.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="172">
   <si>
     <t>COMM1_CD</t>
   </si>
@@ -511,6 +511,30 @@
   </si>
   <si>
     <t>포장공정</t>
+  </si>
+  <si>
+    <t>B80</t>
+  </si>
+  <si>
+    <t>전체공정</t>
+  </si>
+  <si>
+    <t>전처리공정</t>
+  </si>
+  <si>
+    <t>반죽물공정</t>
+  </si>
+  <si>
+    <t>살균공정</t>
+  </si>
+  <si>
+    <t>냉장보관</t>
+  </si>
+  <si>
+    <t>금속검출공정</t>
+  </si>
+  <si>
+    <t>급냉공정</t>
   </si>
 </sst>
 </file>
@@ -840,10 +864,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B144" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2956,6 +2980,397 @@
         <v>20201201153327</v>
       </c>
     </row>
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>164</v>
+      </c>
+      <c r="B125" t="s">
+        <v>6</v>
+      </c>
+      <c r="C125" t="s">
+        <v>165</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125" s="1">
+        <v>20201201153328</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>164</v>
+      </c>
+      <c r="B126">
+        <v>10</v>
+      </c>
+      <c r="C126" t="s">
+        <v>166</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E126" s="1">
+        <v>20201201153329</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>164</v>
+      </c>
+      <c r="B127">
+        <v>15</v>
+      </c>
+      <c r="C127" t="s">
+        <v>107</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E127" s="1">
+        <v>20201201153330</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>164</v>
+      </c>
+      <c r="B128">
+        <v>20</v>
+      </c>
+      <c r="C128" t="s">
+        <v>102</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E128" s="1">
+        <v>20201201153331</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>164</v>
+      </c>
+      <c r="B129">
+        <v>25</v>
+      </c>
+      <c r="C129" t="s">
+        <v>110</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E129" s="1">
+        <v>20201201153332</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>164</v>
+      </c>
+      <c r="B130">
+        <v>30</v>
+      </c>
+      <c r="C130" t="s">
+        <v>105</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E130" s="1">
+        <v>20201201153333</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>164</v>
+      </c>
+      <c r="B131">
+        <v>35</v>
+      </c>
+      <c r="C131" t="s">
+        <v>111</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E131" s="1">
+        <v>20201201153334</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>164</v>
+      </c>
+      <c r="B132">
+        <v>36</v>
+      </c>
+      <c r="C132" t="s">
+        <v>116</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E132" s="1">
+        <v>20201201153335</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>164</v>
+      </c>
+      <c r="B133">
+        <v>37</v>
+      </c>
+      <c r="C133" t="s">
+        <v>167</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E133" s="1">
+        <v>20201201153336</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>164</v>
+      </c>
+      <c r="B134">
+        <v>38</v>
+      </c>
+      <c r="C134" t="s">
+        <v>115</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E134" s="1">
+        <v>20201201153337</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>164</v>
+      </c>
+      <c r="B135">
+        <v>40</v>
+      </c>
+      <c r="C135" t="s">
+        <v>168</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E135" s="1">
+        <v>20201201153338</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>164</v>
+      </c>
+      <c r="B136">
+        <v>45</v>
+      </c>
+      <c r="C136" t="s">
+        <v>103</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E136" s="1">
+        <v>20201201153339</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>164</v>
+      </c>
+      <c r="B137">
+        <v>50</v>
+      </c>
+      <c r="C137" t="s">
+        <v>169</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E137" s="1">
+        <v>20201201153340</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>164</v>
+      </c>
+      <c r="B138">
+        <v>55</v>
+      </c>
+      <c r="C138" t="s">
+        <v>112</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E138" s="1">
+        <v>20201201153341</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>164</v>
+      </c>
+      <c r="B139">
+        <v>60</v>
+      </c>
+      <c r="C139" t="s">
+        <v>104</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E139" s="1">
+        <v>20201201153342</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>164</v>
+      </c>
+      <c r="B140">
+        <v>65</v>
+      </c>
+      <c r="C140" t="s">
+        <v>106</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E140" s="1">
+        <v>20201201153343</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>164</v>
+      </c>
+      <c r="B141">
+        <v>70</v>
+      </c>
+      <c r="C141" t="s">
+        <v>100</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E141" s="1">
+        <v>20201201153344</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>164</v>
+      </c>
+      <c r="B142">
+        <v>75</v>
+      </c>
+      <c r="C142" t="s">
+        <v>113</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E142" s="1">
+        <v>20201201153345</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>164</v>
+      </c>
+      <c r="B143">
+        <v>80</v>
+      </c>
+      <c r="C143" t="s">
+        <v>101</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E143" s="1">
+        <v>20201201153346</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>164</v>
+      </c>
+      <c r="B144">
+        <v>85</v>
+      </c>
+      <c r="C144" t="s">
+        <v>163</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E144" s="1">
+        <v>20201201153347</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>164</v>
+      </c>
+      <c r="B145">
+        <v>90</v>
+      </c>
+      <c r="C145" t="s">
+        <v>170</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E145" s="1">
+        <v>20201201153348</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>164</v>
+      </c>
+      <c r="B146">
+        <v>95</v>
+      </c>
+      <c r="C146" t="s">
+        <v>171</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E146" s="1">
+        <v>20201201153349</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>164</v>
+      </c>
+      <c r="B147">
+        <v>99</v>
+      </c>
+      <c r="C147" t="s">
+        <v>162</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E147" s="1">
+        <v>20201201153350</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new job_ord, job_ord_dtl migrations, models, events and resources added
</commit_message>
<xml_diff>
--- a/database/seeds/common_code.xlsx
+++ b/database/seeds/common_code.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="196">
   <si>
     <t>COMM1_CD</t>
   </si>
@@ -535,6 +535,78 @@
   </si>
   <si>
     <t>급냉공정</t>
+  </si>
+  <si>
+    <t>C00</t>
+  </si>
+  <si>
+    <t>CCP 장비코드</t>
+  </si>
+  <si>
+    <t>CONOVN</t>
+  </si>
+  <si>
+    <t>컨벤션오븐기</t>
+  </si>
+  <si>
+    <t>FREZFS</t>
+  </si>
+  <si>
+    <t>급냉고(반제품)-2</t>
+  </si>
+  <si>
+    <t>FREZMA</t>
+  </si>
+  <si>
+    <t>냉동고(원재료)</t>
+  </si>
+  <si>
+    <t>QUFRE1</t>
+  </si>
+  <si>
+    <t>급냉고(반제품)-1</t>
+  </si>
+  <si>
+    <t>QUFRE2</t>
+  </si>
+  <si>
+    <t>냉동고(완제품)</t>
+  </si>
+  <si>
+    <t>BBMIX1</t>
+  </si>
+  <si>
+    <t>볶음솥+밥혼합기</t>
+  </si>
+  <si>
+    <t>TART1</t>
+  </si>
+  <si>
+    <t>타르트제조용</t>
+  </si>
+  <si>
+    <t>RTEMPS</t>
+  </si>
+  <si>
+    <t>상온저장고(원재료)</t>
+  </si>
+  <si>
+    <t>COOKRM</t>
+  </si>
+  <si>
+    <t>조리실 룸</t>
+  </si>
+  <si>
+    <t>COLDSM</t>
+  </si>
+  <si>
+    <t>저온저장고(원재료)</t>
+  </si>
+  <si>
+    <t>REFRCD</t>
+  </si>
+  <si>
+    <t>냉장고(식힘)</t>
   </si>
 </sst>
 </file>
@@ -864,10 +936,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B144" sqref="B144"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3371,6 +3443,210 @@
         <v>20201201153350</v>
       </c>
     </row>
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>172</v>
+      </c>
+      <c r="B148" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148" t="s">
+        <v>173</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E148" s="1">
+        <v>20201201153351</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>172</v>
+      </c>
+      <c r="B149" t="s">
+        <v>174</v>
+      </c>
+      <c r="C149" t="s">
+        <v>175</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E149" s="1">
+        <v>20201201153352</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>172</v>
+      </c>
+      <c r="B150" t="s">
+        <v>176</v>
+      </c>
+      <c r="C150" t="s">
+        <v>177</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E150" s="1">
+        <v>20201201153353</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>172</v>
+      </c>
+      <c r="B151" t="s">
+        <v>178</v>
+      </c>
+      <c r="C151" t="s">
+        <v>179</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E151" s="1">
+        <v>20201201153354</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>172</v>
+      </c>
+      <c r="B152" t="s">
+        <v>180</v>
+      </c>
+      <c r="C152" t="s">
+        <v>181</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E152" s="1">
+        <v>20201201153355</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>172</v>
+      </c>
+      <c r="B153" t="s">
+        <v>182</v>
+      </c>
+      <c r="C153" t="s">
+        <v>183</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E153" s="1">
+        <v>20201201153356</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>172</v>
+      </c>
+      <c r="B154" t="s">
+        <v>184</v>
+      </c>
+      <c r="C154" t="s">
+        <v>185</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E154" s="1">
+        <v>20201201153357</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>172</v>
+      </c>
+      <c r="B155" t="s">
+        <v>186</v>
+      </c>
+      <c r="C155" t="s">
+        <v>187</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E155" s="1">
+        <v>20201201153358</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>172</v>
+      </c>
+      <c r="B156" t="s">
+        <v>188</v>
+      </c>
+      <c r="C156" t="s">
+        <v>189</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E156" s="1">
+        <v>20201201153359</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>172</v>
+      </c>
+      <c r="B157" t="s">
+        <v>190</v>
+      </c>
+      <c r="C157" t="s">
+        <v>191</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E157" s="1">
+        <v>20201201153360</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>172</v>
+      </c>
+      <c r="B158" t="s">
+        <v>192</v>
+      </c>
+      <c r="C158" t="s">
+        <v>193</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E158" s="1">
+        <v>20201201153361</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>172</v>
+      </c>
+      <c r="B159" t="s">
+        <v>194</v>
+      </c>
+      <c r="C159" t="s">
+        <v>195</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E159" s="1">
+        <v>20201201153362</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
auto heighting on ag-grids added
</commit_message>
<xml_diff>
--- a/database/seeds/common_code.xlsx
+++ b/database/seeds/common_code.xlsx
@@ -938,11 +938,14 @@
   </sheetPr>
   <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B148" sqref="B148"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="F160" sqref="F160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1349,7 +1352,7 @@
         <v>8</v>
       </c>
       <c r="E24" s="1">
-        <v>20201201153328</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1366,7 +1369,7 @@
         <v>8</v>
       </c>
       <c r="E25" s="1">
-        <v>20201201153329</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1383,7 +1386,7 @@
         <v>8</v>
       </c>
       <c r="E26" s="1">
-        <v>20201201153330</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1400,7 +1403,7 @@
         <v>8</v>
       </c>
       <c r="E27" s="1">
-        <v>20201201153331</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3066,7 +3069,7 @@
         <v>8</v>
       </c>
       <c r="E125" s="1">
-        <v>20201201153328</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3083,7 +3086,7 @@
         <v>8</v>
       </c>
       <c r="E126" s="1">
-        <v>20201201153329</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3100,7 +3103,7 @@
         <v>8</v>
       </c>
       <c r="E127" s="1">
-        <v>20201201153330</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3117,7 +3120,7 @@
         <v>8</v>
       </c>
       <c r="E128" s="1">
-        <v>20201201153331</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3134,7 +3137,7 @@
         <v>8</v>
       </c>
       <c r="E129" s="1">
-        <v>20201201153332</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3151,7 +3154,7 @@
         <v>8</v>
       </c>
       <c r="E130" s="1">
-        <v>20201201153333</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3168,7 +3171,7 @@
         <v>8</v>
       </c>
       <c r="E131" s="1">
-        <v>20201201153334</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3185,7 +3188,7 @@
         <v>8</v>
       </c>
       <c r="E132" s="1">
-        <v>20201201153335</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3202,7 +3205,7 @@
         <v>8</v>
       </c>
       <c r="E133" s="1">
-        <v>20201201153336</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3219,7 +3222,7 @@
         <v>8</v>
       </c>
       <c r="E134" s="1">
-        <v>20201201153337</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3236,7 +3239,7 @@
         <v>8</v>
       </c>
       <c r="E135" s="1">
-        <v>20201201153338</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3253,7 +3256,7 @@
         <v>8</v>
       </c>
       <c r="E136" s="1">
-        <v>20201201153339</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3270,7 +3273,7 @@
         <v>8</v>
       </c>
       <c r="E137" s="1">
-        <v>20201201153340</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3287,7 +3290,7 @@
         <v>8</v>
       </c>
       <c r="E138" s="1">
-        <v>20201201153341</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3304,7 +3307,7 @@
         <v>8</v>
       </c>
       <c r="E139" s="1">
-        <v>20201201153342</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3321,7 +3324,7 @@
         <v>8</v>
       </c>
       <c r="E140" s="1">
-        <v>20201201153343</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3338,7 +3341,7 @@
         <v>8</v>
       </c>
       <c r="E141" s="1">
-        <v>20201201153344</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3355,7 +3358,7 @@
         <v>8</v>
       </c>
       <c r="E142" s="1">
-        <v>20201201153345</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3372,7 +3375,7 @@
         <v>8</v>
       </c>
       <c r="E143" s="1">
-        <v>20201201153346</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3389,7 +3392,7 @@
         <v>8</v>
       </c>
       <c r="E144" s="1">
-        <v>20201201153347</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3406,7 +3409,7 @@
         <v>8</v>
       </c>
       <c r="E145" s="1">
-        <v>20201201153348</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3423,7 +3426,7 @@
         <v>8</v>
       </c>
       <c r="E146" s="1">
-        <v>20201201153349</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3440,7 +3443,7 @@
         <v>8</v>
       </c>
       <c r="E147" s="1">
-        <v>20201201153350</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3457,7 +3460,7 @@
         <v>8</v>
       </c>
       <c r="E148" s="1">
-        <v>20201201153351</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3474,7 +3477,7 @@
         <v>8</v>
       </c>
       <c r="E149" s="1">
-        <v>20201201153352</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3491,7 +3494,7 @@
         <v>8</v>
       </c>
       <c r="E150" s="1">
-        <v>20201201153353</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3508,7 +3511,7 @@
         <v>8</v>
       </c>
       <c r="E151" s="1">
-        <v>20201201153354</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3525,7 +3528,7 @@
         <v>8</v>
       </c>
       <c r="E152" s="1">
-        <v>20201201153355</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3542,7 +3545,7 @@
         <v>8</v>
       </c>
       <c r="E153" s="1">
-        <v>20201201153356</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3559,7 +3562,7 @@
         <v>8</v>
       </c>
       <c r="E154" s="1">
-        <v>20201201153357</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3576,7 +3579,7 @@
         <v>8</v>
       </c>
       <c r="E155" s="1">
-        <v>20201201153358</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3593,7 +3596,7 @@
         <v>8</v>
       </c>
       <c r="E156" s="1">
-        <v>20201201153359</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3610,7 +3613,7 @@
         <v>8</v>
       </c>
       <c r="E157" s="1">
-        <v>20201201153360</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3627,7 +3630,7 @@
         <v>8</v>
       </c>
       <c r="E158" s="1">
-        <v>20201201153361</v>
+        <v>20201201153327</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3644,7 +3647,7 @@
         <v>8</v>
       </c>
       <c r="E159" s="1">
-        <v>20201201153362</v>
+        <v>20201201153327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
notifications migration added, some more ccp limit checker fixes
</commit_message>
<xml_diff>
--- a/database/seeds/common_code.xlsx
+++ b/database/seeds/common_code.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\haccp_mes\database\seeds\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="3 Common_codeList" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="228">
   <si>
     <t>COMM1_CD</t>
   </si>
@@ -703,12 +708,27 @@
     <t>창고코드</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>Administrator users</t>
+  </si>
+  <si>
+    <t>Default Administrator</t>
+  </si>
+  <si>
+    <t>kenny</t>
+  </si>
+  <si>
+    <t>Kwon Yoon</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -771,7 +791,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1041,7 +1061,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1052,19 +1072,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E173"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="D179" sqref="D179"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1081,7 +1101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1098,7 +1118,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1115,7 +1135,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1132,7 +1152,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1149,7 +1169,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1166,7 +1186,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1183,7 +1203,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1200,7 +1220,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1217,7 +1237,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1234,7 +1254,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1251,7 +1271,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1268,7 +1288,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1285,7 +1305,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1302,7 +1322,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1319,7 +1339,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1336,7 +1356,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1353,7 +1373,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1370,7 +1390,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1387,7 +1407,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1404,7 +1424,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1421,7 +1441,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1438,7 +1458,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1455,7 +1475,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>121</v>
       </c>
@@ -1472,7 +1492,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>121</v>
       </c>
@@ -1489,7 +1509,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>121</v>
       </c>
@@ -1506,7 +1526,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>121</v>
       </c>
@@ -1523,7 +1543,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -1540,7 +1560,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
@@ -1557,7 +1577,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>31</v>
       </c>
@@ -1574,7 +1594,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -1591,7 +1611,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -1608,7 +1628,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -1625,7 +1645,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -1642,7 +1662,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -1659,7 +1679,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1676,7 +1696,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -1693,7 +1713,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -1710,7 +1730,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -1727,7 +1747,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -1744,7 +1764,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
@@ -1761,7 +1781,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="12.75">
       <c r="A42" s="1" t="s">
         <v>37</v>
       </c>
@@ -1778,7 +1798,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="12.75">
       <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
@@ -1795,7 +1815,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="12.75">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
@@ -1812,7 +1832,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="12.75">
       <c r="A45" s="1" t="s">
         <v>51</v>
       </c>
@@ -1829,7 +1849,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="12.75">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
@@ -1846,7 +1866,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="12.75">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -1863,7 +1883,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="12.75">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
@@ -1880,7 +1900,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="12.75">
       <c r="A49" s="1" t="s">
         <v>51</v>
       </c>
@@ -1897,7 +1917,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="12.75">
       <c r="A50" s="1" t="s">
         <v>63</v>
       </c>
@@ -1914,7 +1934,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="12.75">
       <c r="A51" s="1" t="s">
         <v>63</v>
       </c>
@@ -1931,7 +1951,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="12.75">
       <c r="A52" s="1" t="s">
         <v>63</v>
       </c>
@@ -1948,7 +1968,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="12.75">
       <c r="A53" s="1" t="s">
         <v>63</v>
       </c>
@@ -1965,7 +1985,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="12.75">
       <c r="A54" s="1" t="s">
         <v>63</v>
       </c>
@@ -1982,7 +2002,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="12.75">
       <c r="A55" s="1" t="s">
         <v>63</v>
       </c>
@@ -1999,7 +2019,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="12.75">
       <c r="A56" s="1" t="s">
         <v>71</v>
       </c>
@@ -2016,7 +2036,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="12.75">
       <c r="A57" s="1" t="s">
         <v>71</v>
       </c>
@@ -2033,7 +2053,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="12.75">
       <c r="A58" s="1" t="s">
         <v>71</v>
       </c>
@@ -2050,7 +2070,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="12.75">
       <c r="A59" s="1" t="s">
         <v>71</v>
       </c>
@@ -2067,7 +2087,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="12.75">
       <c r="A60" s="1" t="s">
         <v>71</v>
       </c>
@@ -2084,7 +2104,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="12.75">
       <c r="A61" s="2" t="s">
         <v>130</v>
       </c>
@@ -2101,7 +2121,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="12.75">
       <c r="A62" s="1" t="s">
         <v>130</v>
       </c>
@@ -2118,7 +2138,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="12.75">
       <c r="A63" s="1" t="s">
         <v>130</v>
       </c>
@@ -2135,7 +2155,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="12.75">
       <c r="A64" s="1" t="s">
         <v>130</v>
       </c>
@@ -2152,7 +2172,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="12.75">
       <c r="A65" s="1" t="s">
         <v>130</v>
       </c>
@@ -2169,7 +2189,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="12.75">
       <c r="A66" s="1" t="s">
         <v>138</v>
       </c>
@@ -2186,7 +2206,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="12.75">
       <c r="A67" s="1" t="s">
         <v>138</v>
       </c>
@@ -2203,7 +2223,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="12.75">
       <c r="A68" s="1" t="s">
         <v>138</v>
       </c>
@@ -2220,7 +2240,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="12.75">
       <c r="A69" s="1" t="s">
         <v>138</v>
       </c>
@@ -2237,7 +2257,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="12.75">
       <c r="A70" s="1" t="s">
         <v>138</v>
       </c>
@@ -2254,7 +2274,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="12.75">
       <c r="A71" s="1" t="s">
         <v>138</v>
       </c>
@@ -2271,7 +2291,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="12.75">
       <c r="A72" s="1" t="s">
         <v>138</v>
       </c>
@@ -2288,7 +2308,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="12.75">
       <c r="A73" s="1" t="s">
         <v>138</v>
       </c>
@@ -2305,7 +2325,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="12.75">
       <c r="A74" s="1" t="s">
         <v>138</v>
       </c>
@@ -2322,7 +2342,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="12.75">
       <c r="A75" s="1" t="s">
         <v>154</v>
       </c>
@@ -2339,7 +2359,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="12.75">
       <c r="A76" s="1" t="s">
         <v>154</v>
       </c>
@@ -2356,7 +2376,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="12.75">
       <c r="A77" s="1" t="s">
         <v>154</v>
       </c>
@@ -2373,7 +2393,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="12.75">
       <c r="A78" s="1" t="s">
         <v>154</v>
       </c>
@@ -2390,7 +2410,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="12.75">
       <c r="A79" s="1" t="s">
         <v>154</v>
       </c>
@@ -2407,7 +2427,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="12.75">
       <c r="A80" s="1" t="s">
         <v>159</v>
       </c>
@@ -2424,7 +2444,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="12.75">
       <c r="A81" s="1" t="s">
         <v>159</v>
       </c>
@@ -2441,7 +2461,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="12.75">
       <c r="A82" s="1" t="s">
         <v>159</v>
       </c>
@@ -2458,7 +2478,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="12.75">
       <c r="A83" s="1" t="s">
         <v>159</v>
       </c>
@@ -2475,7 +2495,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="12.75">
       <c r="A84" s="1" t="s">
         <v>72</v>
       </c>
@@ -2492,7 +2512,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="12.75">
       <c r="A85" s="1" t="s">
         <v>72</v>
       </c>
@@ -2509,7 +2529,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="12.75">
       <c r="A86" s="1" t="s">
         <v>72</v>
       </c>
@@ -2526,7 +2546,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="12.75">
       <c r="A87" s="1" t="s">
         <v>72</v>
       </c>
@@ -2543,7 +2563,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="12.75">
       <c r="A88" s="1" t="s">
         <v>72</v>
       </c>
@@ -2560,7 +2580,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="12.75">
       <c r="A89" s="1" t="s">
         <v>72</v>
       </c>
@@ -2577,7 +2597,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="12.75">
       <c r="A90" s="1" t="s">
         <v>79</v>
       </c>
@@ -2594,7 +2614,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="12.75">
       <c r="A91" s="1" t="s">
         <v>79</v>
       </c>
@@ -2611,7 +2631,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="12.75">
       <c r="A92" s="1" t="s">
         <v>79</v>
       </c>
@@ -2628,7 +2648,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="12.75">
       <c r="A93" s="1" t="s">
         <v>79</v>
       </c>
@@ -2645,7 +2665,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="12.75">
       <c r="A94" s="1" t="s">
         <v>79</v>
       </c>
@@ -2662,7 +2682,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="12.75">
       <c r="A95" s="1" t="s">
         <v>79</v>
       </c>
@@ -2679,7 +2699,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="12.75">
       <c r="A96" s="1" t="s">
         <v>90</v>
       </c>
@@ -2696,7 +2716,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="12.75">
       <c r="A97" s="1" t="s">
         <v>90</v>
       </c>
@@ -2713,7 +2733,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="12.75">
       <c r="A98" s="1" t="s">
         <v>90</v>
       </c>
@@ -2730,7 +2750,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="12.75">
       <c r="A99" s="1" t="s">
         <v>90</v>
       </c>
@@ -2747,7 +2767,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="12.75">
       <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
@@ -2764,7 +2784,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="12.75">
       <c r="A101" s="1" t="s">
         <v>98</v>
       </c>
@@ -2781,7 +2801,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="12.75">
       <c r="A102" s="1" t="s">
         <v>98</v>
       </c>
@@ -2798,7 +2818,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="12.75">
       <c r="A103" s="1" t="s">
         <v>98</v>
       </c>
@@ -2815,7 +2835,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="12.75">
       <c r="A104" s="1" t="s">
         <v>98</v>
       </c>
@@ -2832,7 +2852,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="12.75">
       <c r="A105" s="1" t="s">
         <v>98</v>
       </c>
@@ -2849,7 +2869,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="12.75">
       <c r="A106" s="1" t="s">
         <v>98</v>
       </c>
@@ -2866,7 +2886,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="12.75">
       <c r="A107" s="1" t="s">
         <v>98</v>
       </c>
@@ -2883,7 +2903,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="12.75">
       <c r="A108" s="1" t="s">
         <v>98</v>
       </c>
@@ -2900,7 +2920,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="12.75">
       <c r="A109" s="1" t="s">
         <v>108</v>
       </c>
@@ -2917,7 +2937,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="12.75">
       <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
@@ -2934,7 +2954,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="12.75">
       <c r="A111" s="1" t="s">
         <v>108</v>
       </c>
@@ -2951,7 +2971,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="12.75">
       <c r="A112" s="1" t="s">
         <v>108</v>
       </c>
@@ -2968,7 +2988,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="12.75">
       <c r="A113" s="1" t="s">
         <v>108</v>
       </c>
@@ -2985,7 +3005,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="12.75">
       <c r="A114" s="1" t="s">
         <v>108</v>
       </c>
@@ -3002,7 +3022,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="12.75">
       <c r="A115" s="1" t="s">
         <v>108</v>
       </c>
@@ -3019,7 +3039,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="12.75">
       <c r="A116" s="1" t="s">
         <v>108</v>
       </c>
@@ -3036,7 +3056,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="12.75">
       <c r="A117" s="1" t="s">
         <v>108</v>
       </c>
@@ -3053,7 +3073,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="12.75">
       <c r="A118" s="1" t="s">
         <v>108</v>
       </c>
@@ -3070,7 +3090,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="12.75">
       <c r="A119" s="1" t="s">
         <v>108</v>
       </c>
@@ -3087,7 +3107,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="12.75">
       <c r="A120" s="1" t="s">
         <v>108</v>
       </c>
@@ -3104,7 +3124,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="12.75">
       <c r="A121" s="1" t="s">
         <v>117</v>
       </c>
@@ -3121,7 +3141,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="12.75">
       <c r="A122" s="1" t="s">
         <v>117</v>
       </c>
@@ -3138,7 +3158,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="12.75">
       <c r="A123" s="1" t="s">
         <v>117</v>
       </c>
@@ -3155,7 +3175,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="12.75">
       <c r="A124" s="1" t="s">
         <v>117</v>
       </c>
@@ -3172,7 +3192,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1">
       <c r="A125" t="s">
         <v>164</v>
       </c>
@@ -3189,7 +3209,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1">
       <c r="A126" t="s">
         <v>164</v>
       </c>
@@ -3206,7 +3226,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1">
       <c r="A127" t="s">
         <v>164</v>
       </c>
@@ -3223,7 +3243,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1">
       <c r="A128" t="s">
         <v>164</v>
       </c>
@@ -3240,7 +3260,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1">
       <c r="A129" t="s">
         <v>164</v>
       </c>
@@ -3257,7 +3277,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1">
       <c r="A130" t="s">
         <v>164</v>
       </c>
@@ -3274,7 +3294,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1">
       <c r="A131" t="s">
         <v>164</v>
       </c>
@@ -3291,7 +3311,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1">
       <c r="A132" t="s">
         <v>164</v>
       </c>
@@ -3308,7 +3328,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1">
       <c r="A133" t="s">
         <v>164</v>
       </c>
@@ -3325,7 +3345,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1">
       <c r="A134" t="s">
         <v>164</v>
       </c>
@@ -3342,7 +3362,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1">
       <c r="A135" t="s">
         <v>164</v>
       </c>
@@ -3359,7 +3379,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1">
       <c r="A136" t="s">
         <v>164</v>
       </c>
@@ -3376,7 +3396,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1">
       <c r="A137" t="s">
         <v>164</v>
       </c>
@@ -3393,7 +3413,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1">
       <c r="A138" t="s">
         <v>164</v>
       </c>
@@ -3410,7 +3430,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1">
       <c r="A139" t="s">
         <v>164</v>
       </c>
@@ -3427,7 +3447,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1">
       <c r="A140" t="s">
         <v>164</v>
       </c>
@@ -3444,7 +3464,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1">
       <c r="A141" t="s">
         <v>164</v>
       </c>
@@ -3461,7 +3481,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1">
       <c r="A142" t="s">
         <v>164</v>
       </c>
@@ -3478,7 +3498,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1">
       <c r="A143" t="s">
         <v>164</v>
       </c>
@@ -3495,7 +3515,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1">
       <c r="A144" t="s">
         <v>164</v>
       </c>
@@ -3512,7 +3532,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1">
       <c r="A145" t="s">
         <v>164</v>
       </c>
@@ -3529,7 +3549,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1">
       <c r="A146" t="s">
         <v>164</v>
       </c>
@@ -3546,7 +3566,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1">
       <c r="A147" t="s">
         <v>164</v>
       </c>
@@ -3563,7 +3583,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1">
       <c r="A148" t="s">
         <v>172</v>
       </c>
@@ -3580,7 +3600,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1">
       <c r="A149" t="s">
         <v>172</v>
       </c>
@@ -3597,7 +3617,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1">
       <c r="A150" t="s">
         <v>172</v>
       </c>
@@ -3614,7 +3634,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1">
       <c r="A151" t="s">
         <v>172</v>
       </c>
@@ -3631,7 +3651,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1">
       <c r="A152" t="s">
         <v>172</v>
       </c>
@@ -3648,7 +3668,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1">
       <c r="A153" t="s">
         <v>172</v>
       </c>
@@ -3665,7 +3685,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1">
       <c r="A154" t="s">
         <v>172</v>
       </c>
@@ -3682,7 +3702,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1">
       <c r="A155" t="s">
         <v>172</v>
       </c>
@@ -3699,7 +3719,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1">
       <c r="A156" t="s">
         <v>172</v>
       </c>
@@ -3716,7 +3736,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1">
       <c r="A157" t="s">
         <v>172</v>
       </c>
@@ -3733,7 +3753,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1">
       <c r="A158" t="s">
         <v>172</v>
       </c>
@@ -3750,7 +3770,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1">
       <c r="A159" t="s">
         <v>172</v>
       </c>
@@ -3767,7 +3787,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1">
       <c r="A160" t="s">
         <v>196</v>
       </c>
@@ -3784,7 +3804,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1">
       <c r="A161" t="s">
         <v>196</v>
       </c>
@@ -3801,7 +3821,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1">
       <c r="A162" t="s">
         <v>196</v>
       </c>
@@ -3818,7 +3838,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1">
       <c r="A163" s="4" t="s">
         <v>221</v>
       </c>
@@ -3835,7 +3855,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1">
       <c r="A164" s="4" t="s">
         <v>221</v>
       </c>
@@ -3852,7 +3872,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1">
       <c r="A165" s="4" t="s">
         <v>221</v>
       </c>
@@ -3869,7 +3889,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1">
       <c r="A166" s="4" t="s">
         <v>221</v>
       </c>
@@ -3886,7 +3906,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1">
       <c r="A167" s="4" t="s">
         <v>221</v>
       </c>
@@ -3903,7 +3923,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1">
       <c r="A168" s="4" t="s">
         <v>221</v>
       </c>
@@ -3920,7 +3940,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1">
       <c r="A169" s="4" t="s">
         <v>221</v>
       </c>
@@ -3937,7 +3957,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1">
       <c r="A170" s="4" t="s">
         <v>221</v>
       </c>
@@ -3954,7 +3974,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1">
       <c r="A171" s="4" t="s">
         <v>221</v>
       </c>
@@ -3971,7 +3991,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1">
       <c r="A172" s="4" t="s">
         <v>221</v>
       </c>
@@ -3988,7 +4008,7 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1">
       <c r="A173" s="4" t="s">
         <v>221</v>
       </c>
@@ -4002,6 +4022,57 @@
         <v>8</v>
       </c>
       <c r="E173" s="1">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A174" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B174" t="s">
+        <v>6</v>
+      </c>
+      <c r="C174" t="s">
+        <v>224</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E174" s="1">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A175" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B175" t="s">
+        <v>8</v>
+      </c>
+      <c r="C175" t="s">
+        <v>225</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E175" s="1">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A176" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B176" t="s">
+        <v>226</v>
+      </c>
+      <c r="C176" t="s">
+        <v>227</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E176" s="1">
         <v>20201201153327</v>
       </c>
     </row>

</xml_diff>

<commit_message>
print btn, migration and ccp screen changes, removed i18n switcher from navbar
</commit_message>
<xml_diff>
--- a/database/seeds/common_code.xlsx
+++ b/database/seeds/common_code.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="234">
   <si>
     <t>COMM1_CD</t>
   </si>
@@ -722,6 +722,24 @@
   </si>
   <si>
     <t>Kwon Yoon</t>
+  </si>
+  <si>
+    <t>W20</t>
+  </si>
+  <si>
+    <t>CCP 재료코드</t>
+  </si>
+  <si>
+    <t>쌀</t>
+  </si>
+  <si>
+    <t>시금치</t>
+  </si>
+  <si>
+    <t>당근</t>
+  </si>
+  <si>
+    <t>돼지고기</t>
   </si>
 </sst>
 </file>
@@ -783,9 +801,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1072,10 +1094,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E176"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="D179" sqref="D179"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4076,6 +4098,108 @@
         <v>20201201153327</v>
       </c>
     </row>
+    <row r="177" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A177" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B177" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D177" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E177" s="6">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A178" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B178" s="5">
+        <v>10</v>
+      </c>
+      <c r="C178" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D178" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E178" s="6">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A179" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B179" s="5">
+        <v>20</v>
+      </c>
+      <c r="C179" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D179" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E179" s="6">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A180" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B180" s="5">
+        <v>30</v>
+      </c>
+      <c r="C180" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D180" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E180" s="6">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A181" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B181" s="5">
+        <v>40</v>
+      </c>
+      <c r="C181" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D181" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E181" s="6">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A182" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B182" s="5">
+        <v>50</v>
+      </c>
+      <c r="C182" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D182" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E182" s="6">
+        <v>20201201153327</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new ccp_esc_yn, hist table migrations added
</commit_message>
<xml_diff>
--- a/database/seeds/common_code.xlsx
+++ b/database/seeds/common_code.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="237">
   <si>
     <t>COMM1_CD</t>
   </si>
@@ -740,6 +740,71 @@
   </si>
   <si>
     <t>돼지고기</t>
+  </si>
+  <si>
+    <t>소고기</t>
+  </si>
+  <si>
+    <r>
+      <t>알가열제품</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>계란구이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>절임식품</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>단무지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -801,7 +866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -811,6 +876,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1094,10 +1165,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="C177" sqref="C177"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4116,88 +4187,139 @@
       </c>
     </row>
     <row r="178" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A178" s="8" t="s">
+      <c r="A178" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="B178" s="5">
+      <c r="B178" s="12">
         <v>10</v>
       </c>
-      <c r="C178" s="7" t="s">
+      <c r="C178" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="D178" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E178" s="6">
+      <c r="D178" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E178" s="9">
         <v>20201201153327</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A179" s="8" t="s">
+      <c r="A179" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="B179" s="5">
+      <c r="B179" s="12">
         <v>20</v>
       </c>
-      <c r="C179" s="7" t="s">
+      <c r="C179" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="D179" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E179" s="6">
+      <c r="D179" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E179" s="9">
         <v>20201201153327</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A180" s="8" t="s">
+      <c r="A180" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="B180" s="5">
+      <c r="B180" s="12">
         <v>30</v>
       </c>
-      <c r="C180" s="7" t="s">
+      <c r="C180" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="D180" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E180" s="6">
+      <c r="D180" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E180" s="9">
         <v>20201201153327</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A181" s="8" t="s">
+      <c r="A181" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="B181" s="5">
+      <c r="B181" s="12">
         <v>40</v>
       </c>
-      <c r="C181" s="7" t="s">
+      <c r="C181" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D181" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E181" s="6">
+      <c r="D181" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E181" s="9">
         <v>20201201153327</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A182" s="8" t="s">
+      <c r="A182" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="B182" s="5">
+      <c r="B182" s="12">
+        <v>41</v>
+      </c>
+      <c r="C182" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D182" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E182" s="9">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A183" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="B183" s="12">
         <v>50</v>
       </c>
-      <c r="C182" s="7" t="s">
+      <c r="C183" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="D182" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E182" s="6">
-        <v>20201201153327</v>
+      <c r="D183" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E183" s="9">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A184" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="B184" s="12">
+        <v>60</v>
+      </c>
+      <c r="C184" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="D184" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E184" s="9">
+        <v>20201201153328</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A185" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="B185" s="12">
+        <v>70</v>
+      </c>
+      <c r="C185" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="D185" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E185" s="9">
+        <v>20201201153329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worker label & excel convert but not code to name
</commit_message>
<xml_diff>
--- a/database/seeds/common_code.xlsx
+++ b/database/seeds/common_code.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="271">
   <si>
     <t>COMM1_CD</t>
   </si>
@@ -596,23 +596,23 @@
   </si>
   <si>
     <t>컨벡션오븐기</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>C10</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>승인요청</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>승인완료</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>결재승인코드</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>00001</t>
@@ -676,7 +676,7 @@
   </si>
   <si>
     <t>$$</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -691,11 +691,11 @@
       </rPr>
       <t>10</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>창고코드</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>AAA</t>
@@ -916,7 +916,7 @@
       </rPr>
       <t>)</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -957,18 +957,320 @@
       </rPr>
       <t>)</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>상온저장고</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>원재료</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>습도</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조리실</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> ROOM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>습도</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조리실</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> ROOM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>온도</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>상온저장고</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>원재료</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>온도</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>무선탐침봉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> -2</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>무선탐침봉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> -3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>무선탐침봉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> -5</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>무선탐침봉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> -9</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1020,23 +1322,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1309,7 +1612,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1322,13 +1625,13 @@
   </sheetPr>
   <dimension ref="A1:E209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="C150" sqref="C150"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4042,8 +4345,8 @@
       <c r="B160" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="C160" s="13" t="s">
-        <v>235</v>
+      <c r="C160" s="14" t="s">
+        <v>264</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>8</v>
@@ -4059,8 +4362,8 @@
       <c r="B161" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="C161" s="13" t="s">
-        <v>236</v>
+      <c r="C161" s="14" t="s">
+        <v>265</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>8</v>
@@ -4076,8 +4379,8 @@
       <c r="B162" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="C162" s="13" t="s">
-        <v>237</v>
+      <c r="C162" s="14" t="s">
+        <v>263</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>8</v>
@@ -4093,8 +4396,8 @@
       <c r="B163" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="C163" s="13" t="s">
-        <v>238</v>
+      <c r="C163" s="14" t="s">
+        <v>266</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>8</v>
@@ -4144,8 +4447,8 @@
       <c r="B166" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="C166" s="13" t="s">
-        <v>241</v>
+      <c r="C166" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>8</v>
@@ -4154,15 +4457,15 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="167" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A167" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B167" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="C167" s="13" t="s">
-        <v>242</v>
+      <c r="C167" s="14" t="s">
+        <v>268</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>8</v>
@@ -4178,8 +4481,8 @@
       <c r="B168" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="C168" s="13" t="s">
-        <v>243</v>
+      <c r="C168" s="14" t="s">
+        <v>269</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>8</v>
@@ -4195,8 +4498,8 @@
       <c r="B169" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="C169" s="13" t="s">
-        <v>244</v>
+      <c r="C169" s="14" t="s">
+        <v>270</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>8</v>
@@ -4886,7 +5189,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
login hist and user screen required fields updated
</commit_message>
<xml_diff>
--- a/database/seeds/common_code.xlsx
+++ b/database/seeds/common_code.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="275">
   <si>
     <t>COMM1_CD</t>
   </si>
@@ -73,9 +73,6 @@
     <t>구매관리</t>
   </si>
   <si>
-    <t>주문처리</t>
-  </si>
-  <si>
     <t>생산관리</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
   </si>
   <si>
     <t>HACCP모니터링</t>
-  </si>
-  <si>
-    <t>자료관리</t>
   </si>
   <si>
     <t>A20</t>
@@ -1253,12 +1247,47 @@
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>생산관리</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>거래처정보</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고관리</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>자료관리</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>EMP</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>임시저장</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1301,6 +1330,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1322,7 +1357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1340,6 +1375,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1612,7 +1648,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1625,8 +1661,8 @@
   </sheetPr>
   <dimension ref="A1:E209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1795,8 +1831,8 @@
       <c r="B10" s="1">
         <v>20</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
+      <c r="C10" s="15" t="s">
+        <v>269</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -1812,8 +1848,8 @@
       <c r="B11" s="1">
         <v>30</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
+      <c r="C11" s="15" t="s">
+        <v>270</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
@@ -1829,8 +1865,8 @@
       <c r="B12" s="1">
         <v>40</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
+      <c r="C12" s="15" t="s">
+        <v>271</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>8</v>
@@ -1863,8 +1899,8 @@
       <c r="B14" s="1">
         <v>60</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>22</v>
+      <c r="C14" s="15" t="s">
+        <v>272</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
@@ -1875,10 +1911,10 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1">
-        <v>70</v>
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>23</v>
@@ -1892,13 +1928,13 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="B16" s="1">
+        <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>8</v>
@@ -1909,13 +1945,13 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>8</v>
@@ -1926,13 +1962,13 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B18" s="1">
-        <v>20</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
@@ -1943,13 +1979,13 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>8</v>
@@ -1960,13 +1996,13 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="1">
-        <v>40</v>
+        <v>25</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>8</v>
@@ -1977,13 +2013,13 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>8</v>
@@ -1994,13 +2030,13 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>8</v>
@@ -2011,13 +2047,13 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="1">
-        <v>20</v>
+        <v>119</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
@@ -2027,14 +2063,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="1">
+        <v>10</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>8</v>
@@ -2045,13 +2081,13 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B25" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>123</v>
+        <v>34</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>8</v>
@@ -2062,13 +2098,13 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B26" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
@@ -2078,15 +2114,15 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B27" s="1">
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
@@ -2095,11 +2131,11 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>6</v>
+      <c r="A28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="1">
+        <v>10</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -2113,10 +2149,10 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>34</v>
@@ -2129,11 +2165,11 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>31</v>
+      <c r="A30" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>36</v>
@@ -2149,11 +2185,11 @@
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="1">
-        <v>30</v>
+      <c r="B31" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>8</v>
@@ -2164,13 +2200,13 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>10</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
@@ -2181,13 +2217,13 @@
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
@@ -2198,13 +2234,13 @@
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B34" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>8</v>
@@ -2217,11 +2253,11 @@
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="1">
-        <v>30</v>
+      <c r="B35" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>8</v>
@@ -2232,13 +2268,13 @@
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
+      </c>
+      <c r="B36" s="1">
+        <v>10</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>8</v>
@@ -2249,13 +2285,13 @@
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B37" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>8</v>
@@ -2266,13 +2302,13 @@
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B38" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>8</v>
@@ -2285,11 +2321,11 @@
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="1">
-        <v>30</v>
+      <c r="B39" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>8</v>
@@ -2300,30 +2336,30 @@
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
+      </c>
+      <c r="B40" s="1">
+        <v>10</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="1">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="1">
+        <v>20</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="1">
-        <v>20201201153327</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="1">
-        <v>10</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>8</v>
@@ -2334,13 +2370,13 @@
     </row>
     <row r="42" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B42" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>8</v>
@@ -2351,10 +2387,10 @@
     </row>
     <row r="43" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="1">
-        <v>30</v>
+        <v>49</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>50</v>
@@ -2368,10 +2404,10 @@
     </row>
     <row r="44" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>52</v>
@@ -2385,7 +2421,7 @@
     </row>
     <row r="45" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>53</v>
@@ -2402,7 +2438,7 @@
     </row>
     <row r="46" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>55</v>
@@ -2419,7 +2455,7 @@
     </row>
     <row r="47" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>57</v>
@@ -2436,7 +2472,7 @@
     </row>
     <row r="48" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>59</v>
@@ -2453,10 +2489,10 @@
     </row>
     <row r="49" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>62</v>
@@ -2470,10 +2506,10 @@
     </row>
     <row r="50" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>64</v>
@@ -2487,7 +2523,7 @@
     </row>
     <row r="51" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>65</v>
@@ -2504,13 +2540,13 @@
     </row>
     <row r="52" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>8</v>
@@ -2521,13 +2557,13 @@
     </row>
     <row r="53" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>8</v>
@@ -2538,13 +2574,13 @@
     </row>
     <row r="54" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>8</v>
@@ -2555,13 +2591,13 @@
     </row>
     <row r="55" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>8</v>
@@ -2572,13 +2608,13 @@
     </row>
     <row r="56" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>6</v>
+        <v>69</v>
+      </c>
+      <c r="B56" s="1">
+        <v>10</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>8</v>
@@ -2589,13 +2625,13 @@
     </row>
     <row r="57" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B57" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>8</v>
@@ -2606,13 +2642,13 @@
     </row>
     <row r="58" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B58" s="1">
-        <v>20</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>127</v>
+        <v>30</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>8</v>
@@ -2623,27 +2659,27 @@
     </row>
     <row r="59" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B59" s="1">
-        <v>30</v>
-      </c>
-      <c r="C59" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="1">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" s="1">
-        <v>20201201153327</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B60" s="1">
-        <v>40</v>
+      <c r="B60" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>129</v>
@@ -2656,14 +2692,14 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C61" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>8</v>
@@ -2674,13 +2710,13 @@
     </row>
     <row r="62" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>8</v>
@@ -2691,7 +2727,7 @@
     </row>
     <row r="63" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>133</v>
@@ -2708,13 +2744,13 @@
     </row>
     <row r="64" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>8</v>
@@ -2725,10 +2761,10 @@
     </row>
     <row r="65" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>137</v>
@@ -2742,10 +2778,10 @@
     </row>
     <row r="66" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>139</v>
@@ -2759,7 +2795,7 @@
     </row>
     <row r="67" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>140</v>
@@ -2776,7 +2812,7 @@
     </row>
     <row r="68" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>142</v>
@@ -2793,7 +2829,7 @@
     </row>
     <row r="69" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>144</v>
@@ -2810,13 +2846,13 @@
     </row>
     <row r="70" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>146</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>8</v>
@@ -2827,13 +2863,13 @@
     </row>
     <row r="71" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>8</v>
@@ -2844,7 +2880,7 @@
     </row>
     <row r="72" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>149</v>
@@ -2861,13 +2897,13 @@
     </row>
     <row r="73" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>151</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>8</v>
@@ -2878,13 +2914,13 @@
     </row>
     <row r="74" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>8</v>
@@ -2895,13 +2931,13 @@
     </row>
     <row r="75" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>8</v>
@@ -2912,13 +2948,13 @@
     </row>
     <row r="76" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>8</v>
@@ -2929,13 +2965,13 @@
     </row>
     <row r="77" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>142</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>8</v>
@@ -2946,13 +2982,13 @@
     </row>
     <row r="78" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>144</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>8</v>
@@ -2963,13 +2999,13 @@
     </row>
     <row r="79" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>146</v>
+        <v>6</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>8</v>
@@ -2980,13 +3016,13 @@
     </row>
     <row r="80" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" s="1">
+        <v>10</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>8</v>
@@ -2997,13 +3033,13 @@
     </row>
     <row r="81" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B81" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>8</v>
@@ -3014,13 +3050,13 @@
     </row>
     <row r="82" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B82" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>8</v>
@@ -3031,13 +3067,13 @@
     </row>
     <row r="83" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B83" s="1">
-        <v>30</v>
+        <v>70</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>8</v>
@@ -3048,13 +3084,13 @@
     </row>
     <row r="84" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B84" s="1">
+        <v>10</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>8</v>
@@ -3065,13 +3101,13 @@
     </row>
     <row r="85" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B85" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>8</v>
@@ -3082,13 +3118,13 @@
     </row>
     <row r="86" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B86" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>8</v>
@@ -3099,13 +3135,13 @@
     </row>
     <row r="87" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B87" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>8</v>
@@ -3116,13 +3152,13 @@
     </row>
     <row r="88" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B88" s="1">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>8</v>
@@ -3133,10 +3169,10 @@
     </row>
     <row r="89" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B89" s="1">
-        <v>50</v>
+        <v>77</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>78</v>
@@ -3150,10 +3186,10 @@
     </row>
     <row r="90" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>80</v>
@@ -3167,7 +3203,7 @@
     </row>
     <row r="91" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>81</v>
@@ -3184,7 +3220,7 @@
     </row>
     <row r="92" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>83</v>
@@ -3201,7 +3237,7 @@
     </row>
     <row r="93" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>85</v>
@@ -3218,13 +3254,13 @@
     </row>
     <row r="94" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>8</v>
@@ -3235,10 +3271,10 @@
     </row>
     <row r="95" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>89</v>
@@ -3252,10 +3288,10 @@
     </row>
     <row r="96" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>91</v>
@@ -3269,7 +3305,7 @@
     </row>
     <row r="97" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>92</v>
@@ -3286,7 +3322,7 @@
     </row>
     <row r="98" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>94</v>
@@ -3303,10 +3339,10 @@
     </row>
     <row r="99" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>97</v>
@@ -3320,13 +3356,13 @@
     </row>
     <row r="100" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B100" s="1">
+        <v>10</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>8</v>
@@ -3337,13 +3373,13 @@
     </row>
     <row r="101" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B101" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>8</v>
@@ -3354,13 +3390,13 @@
     </row>
     <row r="102" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B102" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>8</v>
@@ -3371,13 +3407,13 @@
     </row>
     <row r="103" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B103" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>8</v>
@@ -3388,13 +3424,13 @@
     </row>
     <row r="104" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B104" s="1">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>8</v>
@@ -3405,13 +3441,13 @@
     </row>
     <row r="105" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B105" s="1">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>8</v>
@@ -3422,13 +3458,13 @@
     </row>
     <row r="106" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B106" s="1">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>8</v>
@@ -3439,13 +3475,13 @@
     </row>
     <row r="107" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B107" s="1">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>8</v>
@@ -3456,10 +3492,10 @@
     </row>
     <row r="108" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B108" s="1">
-        <v>80</v>
+        <v>106</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>107</v>
@@ -3473,13 +3509,13 @@
     </row>
     <row r="109" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B109" s="1">
+        <v>10</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>8</v>
@@ -3490,13 +3526,13 @@
     </row>
     <row r="110" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B110" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>8</v>
@@ -3507,13 +3543,13 @@
     </row>
     <row r="111" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B111" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>8</v>
@@ -3524,13 +3560,13 @@
     </row>
     <row r="112" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B112" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>8</v>
@@ -3541,13 +3577,13 @@
     </row>
     <row r="113" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B113" s="1">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>8</v>
@@ -3558,13 +3594,13 @@
     </row>
     <row r="114" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B114" s="1">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>8</v>
@@ -3575,13 +3611,13 @@
     </row>
     <row r="115" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B115" s="1">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>8</v>
@@ -3592,13 +3628,13 @@
     </row>
     <row r="116" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B116" s="1">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>8</v>
@@ -3609,13 +3645,13 @@
     </row>
     <row r="117" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B117" s="1">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>8</v>
@@ -3626,13 +3662,13 @@
     </row>
     <row r="118" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B118" s="1">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>8</v>
@@ -3643,13 +3679,13 @@
     </row>
     <row r="119" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B119" s="1">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>8</v>
@@ -3660,10 +3696,10 @@
     </row>
     <row r="120" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B120" s="1">
-        <v>95</v>
+        <v>115</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>116</v>
@@ -3677,13 +3713,13 @@
     </row>
     <row r="121" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B121" s="1">
+        <v>10</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>8</v>
@@ -3694,13 +3730,13 @@
     </row>
     <row r="122" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B122" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>8</v>
@@ -3711,13 +3747,13 @@
     </row>
     <row r="123" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B123" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>8</v>
@@ -3726,15 +3762,15 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B124" s="1">
-        <v>30</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>62</v>
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>162</v>
+      </c>
+      <c r="B124" t="s">
+        <v>6</v>
+      </c>
+      <c r="C124" t="s">
+        <v>163</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>8</v>
@@ -3745,13 +3781,13 @@
     </row>
     <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>162</v>
+      </c>
+      <c r="B125">
+        <v>10</v>
+      </c>
+      <c r="C125" t="s">
         <v>164</v>
-      </c>
-      <c r="B125" t="s">
-        <v>6</v>
-      </c>
-      <c r="C125" t="s">
-        <v>165</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>8</v>
@@ -3762,13 +3798,13 @@
     </row>
     <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B126">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C126" t="s">
-        <v>166</v>
+        <v>105</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>8</v>
@@ -3779,13 +3815,13 @@
     </row>
     <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B127">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C127" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>8</v>
@@ -3796,13 +3832,13 @@
     </row>
     <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B128">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C128" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>8</v>
@@ -3813,13 +3849,13 @@
     </row>
     <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B129">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C129" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>8</v>
@@ -3830,13 +3866,13 @@
     </row>
     <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B130">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C130" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>8</v>
@@ -3847,13 +3883,13 @@
     </row>
     <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B131">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C131" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>8</v>
@@ -3864,13 +3900,13 @@
     </row>
     <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B132">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C132" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>8</v>
@@ -3881,13 +3917,13 @@
     </row>
     <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B133">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C133" t="s">
-        <v>167</v>
+        <v>113</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>8</v>
@@ -3898,13 +3934,13 @@
     </row>
     <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B134">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C134" t="s">
-        <v>115</v>
+        <v>166</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>8</v>
@@ -3915,13 +3951,13 @@
     </row>
     <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B135">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C135" t="s">
-        <v>168</v>
+        <v>101</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>8</v>
@@ -3932,13 +3968,13 @@
     </row>
     <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B136">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C136" t="s">
-        <v>103</v>
+        <v>167</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>8</v>
@@ -3949,13 +3985,13 @@
     </row>
     <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B137">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C137" t="s">
-        <v>169</v>
+        <v>110</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>8</v>
@@ -3966,13 +4002,13 @@
     </row>
     <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B138">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C138" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>8</v>
@@ -3983,10 +4019,10 @@
     </row>
     <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B139">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C139" t="s">
         <v>104</v>
@@ -4000,13 +4036,13 @@
     </row>
     <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B140">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C140" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>8</v>
@@ -4017,13 +4053,13 @@
     </row>
     <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B141">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C141" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>8</v>
@@ -4034,13 +4070,13 @@
     </row>
     <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B142">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C142" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>8</v>
@@ -4051,13 +4087,13 @@
     </row>
     <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B143">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C143" t="s">
-        <v>101</v>
+        <v>161</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>8</v>
@@ -4068,13 +4104,13 @@
     </row>
     <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B144">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C144" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>8</v>
@@ -4085,13 +4121,13 @@
     </row>
     <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B145">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C145" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>8</v>
@@ -4102,13 +4138,13 @@
     </row>
     <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B146">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C146" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>8</v>
@@ -4119,13 +4155,13 @@
     </row>
     <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>164</v>
-      </c>
-      <c r="B147">
-        <v>99</v>
+        <v>170</v>
+      </c>
+      <c r="B147" t="s">
+        <v>6</v>
       </c>
       <c r="C147" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>8</v>
@@ -4136,13 +4172,13 @@
     </row>
     <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>170</v>
+      </c>
+      <c r="B148" t="s">
         <v>172</v>
       </c>
-      <c r="B148" t="s">
-        <v>6</v>
-      </c>
-      <c r="C148" t="s">
-        <v>173</v>
+      <c r="C148" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>8</v>
@@ -4153,13 +4189,13 @@
     </row>
     <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B149" t="s">
-        <v>174</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>193</v>
+        <v>173</v>
+      </c>
+      <c r="C149" s="11" t="s">
+        <v>260</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>8</v>
@@ -4170,13 +4206,13 @@
     </row>
     <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B150" t="s">
+        <v>174</v>
+      </c>
+      <c r="C150" t="s">
         <v>175</v>
-      </c>
-      <c r="C150" s="11" t="s">
-        <v>262</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>8</v>
@@ -4187,13 +4223,13 @@
     </row>
     <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B151" t="s">
         <v>176</v>
       </c>
-      <c r="C151" t="s">
-        <v>177</v>
+      <c r="C151" s="11" t="s">
+        <v>259</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>8</v>
@@ -4204,13 +4240,13 @@
     </row>
     <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B152" t="s">
+        <v>177</v>
+      </c>
+      <c r="C152" t="s">
         <v>178</v>
-      </c>
-      <c r="C152" s="11" t="s">
-        <v>261</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>8</v>
@@ -4221,7 +4257,7 @@
     </row>
     <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B153" t="s">
         <v>179</v>
@@ -4238,7 +4274,7 @@
     </row>
     <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B154" t="s">
         <v>181</v>
@@ -4255,7 +4291,7 @@
     </row>
     <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B155" t="s">
         <v>183</v>
@@ -4272,7 +4308,7 @@
     </row>
     <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B156" t="s">
         <v>185</v>
@@ -4289,7 +4325,7 @@
     </row>
     <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B157" t="s">
         <v>187</v>
@@ -4306,7 +4342,7 @@
     </row>
     <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B158" t="s">
         <v>189</v>
@@ -4321,15 +4357,15 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>172</v>
-      </c>
-      <c r="B159" t="s">
-        <v>191</v>
-      </c>
-      <c r="C159" t="s">
-        <v>192</v>
+    <row r="159" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B159" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C159" s="14" t="s">
+        <v>262</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>8</v>
@@ -4340,13 +4376,13 @@
     </row>
     <row r="160" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>8</v>
@@ -4357,13 +4393,13 @@
     </row>
     <row r="161" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C161" s="14" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>8</v>
@@ -4374,13 +4410,13 @@
     </row>
     <row r="162" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C162" s="14" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>8</v>
@@ -4391,13 +4427,13 @@
     </row>
     <row r="163" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B163" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="C163" s="14" t="s">
-        <v>266</v>
+        <v>170</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>8</v>
@@ -4408,13 +4444,13 @@
     </row>
     <row r="164" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B164" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C164" s="5" t="s">
-        <v>239</v>
+        <v>170</v>
+      </c>
+      <c r="B164" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C164" s="13" t="s">
+        <v>238</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>8</v>
@@ -4425,47 +4461,47 @@
     </row>
     <row r="165" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B165" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C165" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E165" s="1">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A166" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B166" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="C165" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E165" s="1">
-        <v>20201201153327</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B166" s="13" t="s">
+      <c r="C166" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E166" s="1">
+        <v>20201201153327</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B167" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="C166" s="14" t="s">
+      <c r="C167" s="14" t="s">
         <v>267</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E166" s="1">
-        <v>20201201153327</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A167" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B167" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="C167" s="14" t="s">
-        <v>268</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>8</v>
@@ -4476,13 +4512,13 @@
     </row>
     <row r="168" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B168" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C168" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>8</v>
@@ -4491,15 +4527,15 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="169" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B169" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="C169" s="14" t="s">
-        <v>270</v>
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>192</v>
+      </c>
+      <c r="B169" t="s">
+        <v>6</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>8</v>
@@ -4510,13 +4546,13 @@
     </row>
     <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>194</v>
-      </c>
-      <c r="B170" t="s">
-        <v>6</v>
+        <v>192</v>
+      </c>
+      <c r="B170">
+        <v>10</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>8</v>
@@ -4527,14 +4563,14 @@
     </row>
     <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>192</v>
+      </c>
+      <c r="B171">
+        <v>20</v>
+      </c>
+      <c r="C171" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B171">
-        <v>10</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>195</v>
-      </c>
       <c r="D171" s="1" t="s">
         <v>8</v>
       </c>
@@ -4542,15 +4578,15 @@
         <v>20201201153327</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>194</v>
-      </c>
-      <c r="B172">
-        <v>20</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>196</v>
+    <row r="172" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B172" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="C172" s="10" t="s">
+        <v>274</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>8</v>
@@ -4561,13 +4597,13 @@
     </row>
     <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B173" t="s">
+        <v>216</v>
+      </c>
+      <c r="C173" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>220</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>8</v>
@@ -4578,13 +4614,13 @@
     </row>
     <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B174" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C174" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>8</v>
@@ -4595,13 +4631,13 @@
     </row>
     <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B175" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C175" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D175" s="1" t="s">
         <v>8</v>
@@ -4612,13 +4648,13 @@
     </row>
     <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B176" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C176" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>8</v>
@@ -4629,13 +4665,13 @@
     </row>
     <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B177" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C177" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D177" s="1" t="s">
         <v>8</v>
@@ -4646,13 +4682,13 @@
     </row>
     <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B178" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C178" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>8</v>
@@ -4663,13 +4699,13 @@
     </row>
     <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B179" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C179" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>8</v>
@@ -4680,13 +4716,13 @@
     </row>
     <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B180" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C180" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>8</v>
@@ -4697,13 +4733,13 @@
     </row>
     <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B181" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C181" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>8</v>
@@ -4714,13 +4750,13 @@
     </row>
     <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B182" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C182" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>8</v>
@@ -4731,13 +4767,13 @@
     </row>
     <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B183" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C183" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>8</v>
@@ -4748,13 +4784,13 @@
     </row>
     <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B184" t="s">
         <v>6</v>
       </c>
       <c r="C184" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>8</v>
@@ -4765,13 +4801,13 @@
     </row>
     <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B185" t="s">
+        <v>8</v>
+      </c>
+      <c r="C185" t="s">
         <v>221</v>
-      </c>
-      <c r="B185" t="s">
-        <v>8</v>
-      </c>
-      <c r="C185" t="s">
-        <v>223</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>8</v>
@@ -4782,13 +4818,13 @@
     </row>
     <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B186" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C186" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>8</v>
@@ -4799,13 +4835,13 @@
     </row>
     <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B187" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C187" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D187" s="6" t="s">
         <v>8</v>
@@ -4816,13 +4852,13 @@
     </row>
     <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B188" s="12">
         <v>10</v>
       </c>
       <c r="C188" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D188" s="9" t="s">
         <v>8</v>
@@ -4833,13 +4869,13 @@
     </row>
     <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B189" s="12">
         <v>20</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D189" s="9" t="s">
         <v>8</v>
@@ -4850,13 +4886,13 @@
     </row>
     <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B190" s="12">
         <v>30</v>
       </c>
       <c r="C190" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D190" s="9" t="s">
         <v>8</v>
@@ -4867,13 +4903,13 @@
     </row>
     <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B191" s="12">
         <v>40</v>
       </c>
       <c r="C191" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D191" s="9" t="s">
         <v>8</v>
@@ -4884,13 +4920,13 @@
     </row>
     <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B192" s="12">
         <v>41</v>
       </c>
       <c r="C192" s="10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D192" s="9" t="s">
         <v>8</v>
@@ -4901,13 +4937,13 @@
     </row>
     <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B193" s="12">
         <v>50</v>
       </c>
       <c r="C193" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D193" s="9" t="s">
         <v>8</v>
@@ -4918,13 +4954,13 @@
     </row>
     <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B194" s="12">
         <v>60</v>
       </c>
       <c r="C194" s="10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D194" s="9" t="s">
         <v>8</v>
@@ -4935,13 +4971,13 @@
     </row>
     <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B195" s="12">
         <v>70</v>
       </c>
       <c r="C195" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>8</v>
@@ -4952,13 +4988,13 @@
     </row>
     <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B196" t="s">
         <v>6</v>
       </c>
       <c r="C196" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D196" s="9" t="s">
         <v>8</v>
@@ -4969,13 +5005,13 @@
     </row>
     <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B197">
         <v>50</v>
       </c>
       <c r="C197" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D197" s="9" t="s">
         <v>8</v>
@@ -4986,13 +5022,13 @@
     </row>
     <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B198">
         <v>60</v>
       </c>
       <c r="C198" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D198" s="9" t="s">
         <v>8</v>
@@ -5003,13 +5039,13 @@
     </row>
     <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B199">
         <v>40</v>
       </c>
       <c r="C199" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D199" s="9" t="s">
         <v>8</v>
@@ -5020,13 +5056,13 @@
     </row>
     <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B200">
         <v>30</v>
       </c>
       <c r="C200" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D200" s="9" t="s">
         <v>8</v>
@@ -5037,13 +5073,13 @@
     </row>
     <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B201">
         <v>10</v>
       </c>
       <c r="C201" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D201" s="9" t="s">
         <v>8</v>
@@ -5054,13 +5090,13 @@
     </row>
     <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B202">
         <v>20</v>
       </c>
       <c r="C202" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D202" s="9" t="s">
         <v>8</v>
@@ -5071,13 +5107,13 @@
     </row>
     <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B203" t="s">
         <v>6</v>
       </c>
       <c r="C203" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D203" s="9" t="s">
         <v>8</v>
@@ -5088,13 +5124,13 @@
     </row>
     <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B204">
         <v>10</v>
       </c>
       <c r="C204" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D204" s="9" t="s">
         <v>8</v>
@@ -5105,13 +5141,13 @@
     </row>
     <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B205">
         <v>20</v>
       </c>
       <c r="C205" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D205" s="9" t="s">
         <v>8</v>
@@ -5122,13 +5158,13 @@
     </row>
     <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B206">
         <v>30</v>
       </c>
       <c r="C206" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D206" s="9" t="s">
         <v>8</v>
@@ -5139,13 +5175,13 @@
     </row>
     <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B207">
         <v>40</v>
       </c>
       <c r="C207" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D207" s="9" t="s">
         <v>8</v>
@@ -5156,13 +5192,13 @@
     </row>
     <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B208">
         <v>50</v>
       </c>
       <c r="C208" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D208" s="9" t="s">
         <v>8</v>
@@ -5173,13 +5209,13 @@
     </row>
     <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B209">
         <v>60</v>
       </c>
       <c r="C209" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D209" s="9" t="s">
         <v>8</v>

</xml_diff>